<commit_message>
Tabell i 04-study..., + git add -A
</commit_message>
<xml_diff>
--- a/plot_data_all_gr.xlsx
+++ b/plot_data_all_gr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IDR4000\mappeeksamen idr4000\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IDR4000\mappeeksamen_idr4000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD0AD38-FAA4-4BA8-A82B-C184DAB41C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D0DFD8-0C75-47F1-8D84-D64AEFD20A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,17 +220,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,2606 +547,2606 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
         <v>17.899999999999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>69</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
         <v>36</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <v>178</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <v>97.5</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="5">
         <v>240.33333333333334</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5">
         <v>3381.5</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5">
         <v>3990.5</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5">
         <v>1.18</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5">
         <v>135</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5">
         <v>42.5</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5">
         <v>175</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5">
         <v>14.2</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
         <v>18.5</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>68</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6">
         <v>36</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <v>178</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <v>97.4</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>230</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6">
         <v>3065</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6">
         <v>3646.5</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6">
         <v>1.19</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6">
         <v>128.5</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6">
         <v>39.450000000000003</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S6" s="3">
+      <c r="R6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6">
         <v>14.23</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
         <v>17.899999999999999</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>69</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7">
         <v>36</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <v>178</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <v>96.6</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>240</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7">
         <v>3190</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7">
         <v>3846.5</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7">
         <v>1.2050000000000001</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7">
         <v>121</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7">
         <v>36.75</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="3">
+      <c r="R7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7">
         <v>14.2</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
         <v>18.7</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>44</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8">
         <v>36</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <v>178</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <v>96.5</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>260.33333333333331</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8">
         <v>3343</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8">
         <v>3946</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8">
         <v>1.18</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8">
         <v>130.5</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8">
         <v>41.9</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8">
         <v>175</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8">
         <v>13.63</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
         <v>18.2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>70</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>24</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <v>162</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9">
         <v>61.9</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>221.66666666666666</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9">
         <v>2771</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9">
         <v>3207.5</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9">
         <v>1.1549999999999998</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9">
         <v>128</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9">
         <v>69.25</v>
       </c>
-      <c r="R9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="3">
+      <c r="R9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9">
         <v>14.01</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
         <v>18.3</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <v>67</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10">
         <v>24</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10">
         <v>162</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <v>61.5</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>220.33333333333334</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10">
         <v>2801.5</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10">
         <v>3299</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10">
         <v>1.18</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10">
         <v>130</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10">
         <v>73.550000000000011</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10">
         <v>185</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10">
         <v>15.23</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11">
         <v>18.2</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <v>70</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11">
         <v>24</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11">
         <v>162</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11">
         <v>61.9</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>217.66666666666666</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11">
         <v>2464.5</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11">
         <v>2945</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11">
         <v>1.1949999999999998</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11">
         <v>115.5</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11">
         <v>66.650000000000006</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11">
         <v>183</v>
       </c>
-      <c r="S11" s="3">
+      <c r="S11">
         <v>12.99</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12">
         <v>19</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <v>45</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12">
         <v>24</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12">
         <v>162</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12">
         <v>61.9</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12">
         <v>224.33333333333334</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12">
         <v>2760</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12">
         <v>3233.5</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12">
         <v>1.17</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12">
         <v>134.5</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12">
         <v>73.5</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12">
         <v>189</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12">
         <v>15.96</v>
       </c>
-      <c r="T12" s="3">
+      <c r="T12">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13">
         <v>18.3</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>70</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13">
         <v>24</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13">
         <v>180</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13">
         <v>79.900000000000006</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13">
         <v>320.33333333333331</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13">
         <v>4234.5</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13">
         <v>4809.5</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13">
         <v>1.1349999999999998</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13">
         <v>168</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13">
         <v>42.45</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13">
         <v>183</v>
       </c>
-      <c r="S13" s="3">
+      <c r="S13">
         <v>12.8</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14">
         <v>18.3</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <v>70</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14">
         <v>24</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14">
         <v>180</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14">
         <v>79.900000000000006</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14">
         <v>310</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14">
         <v>4235</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14">
         <v>4778</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14">
         <v>1.125</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14">
         <v>165.5</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14">
         <v>43.05</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14">
         <v>189</v>
       </c>
-      <c r="S14" s="3">
+      <c r="S14">
         <v>14.61</v>
       </c>
-      <c r="T14" s="3">
+      <c r="T14">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15">
         <v>18.3</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15">
         <v>70</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15">
         <v>24</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15">
         <v>180</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15">
         <v>80.900000000000006</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15">
         <v>241</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15">
         <v>3693.5</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15">
         <v>4119.5</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15">
         <v>1.1150000000000002</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15">
         <v>138.5</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15">
         <v>37.150000000000006</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15">
         <v>175</v>
       </c>
-      <c r="S15" s="3">
+      <c r="S15">
         <v>10.99</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16">
         <v>19.100000000000001</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16">
         <v>46</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16">
         <v>24</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16">
         <v>180</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16">
         <v>79.599999999999994</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="3">
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16">
         <v>4361</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16">
         <v>5056.5</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16">
         <v>1.1599999999999999</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16">
         <v>192</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16">
         <v>49</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16">
         <v>190</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16">
         <v>15.11</v>
       </c>
-      <c r="T16" s="3">
+      <c r="T16">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="D17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17">
         <v>19.899999999999999</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17">
         <v>77</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="3">
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17">
         <v>27</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17">
         <v>176</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17">
         <v>77.599999999999994</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="5">
         <v>222</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17">
         <v>2819.5</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17">
         <v>3595.5</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17">
         <v>1.2749999999999999</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17">
         <v>146</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17">
         <v>64.2</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S17" s="8">
+      <c r="R17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" s="6">
         <v>14.51</v>
       </c>
-      <c r="T17" s="3">
+      <c r="T17">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18">
         <v>19.5</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <v>53</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="3">
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18">
         <v>27</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18">
         <v>176</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18">
         <v>76.400000000000006</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>240</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M18">
         <v>2893</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18">
         <v>3519.5</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18">
         <v>1.2250000000000001</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18">
         <v>160</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="Q18">
         <v>69.2</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18">
         <v>183</v>
       </c>
-      <c r="S18" s="3">
+      <c r="S18">
         <v>16.14</v>
       </c>
-      <c r="T18" s="3">
+      <c r="T18">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="D19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19">
         <v>18.8</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>66</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="3">
-        <v>23</v>
-      </c>
-      <c r="J19" s="3">
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19">
+        <v>23</v>
+      </c>
+      <c r="J19">
         <v>180</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19">
         <v>74.599999999999994</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="5">
         <v>391</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19">
         <v>4427</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19">
         <v>4981</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19">
         <v>1.125</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19">
         <v>161.5</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19">
         <v>56.75</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19">
         <v>203</v>
       </c>
-      <c r="S19" s="8">
+      <c r="S19" s="6">
         <v>13.07</v>
       </c>
-      <c r="T19" s="3">
+      <c r="T19">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="D20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20">
         <v>19.100000000000001</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20">
         <v>68</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="3">
-        <v>23</v>
-      </c>
-      <c r="J20" s="3">
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20">
+        <v>23</v>
+      </c>
+      <c r="J20">
         <v>180</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20">
         <v>74.599999999999994</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="5">
         <v>382.33333333333331</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20">
         <v>4359.5</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20">
         <v>4856.5</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20">
         <v>1.1100000000000001</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20">
         <v>159</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20">
         <v>57.599999999999994</v>
       </c>
-      <c r="R20" s="3">
+      <c r="R20">
         <v>200</v>
       </c>
-      <c r="S20" s="8">
+      <c r="S20" s="6">
         <v>12.26</v>
       </c>
-      <c r="T20" s="3">
+      <c r="T20">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="D21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
         <v>19.399999999999999</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21">
         <v>68</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="3">
-        <v>23</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="I21">
+        <v>23</v>
+      </c>
+      <c r="J21">
         <v>178</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21">
         <v>81.400000000000006</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="5">
         <v>291.33333333333331</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21">
         <v>3713.5</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21">
         <v>4200</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21">
         <v>83.9</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21">
         <v>191</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R21">
         <v>194</v>
       </c>
-      <c r="S21" s="8">
+      <c r="S21" s="6">
         <v>13.43</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T21">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="3">
+      <c r="D22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22">
         <v>19.399999999999999</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22">
         <v>65</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="3">
-        <v>23</v>
-      </c>
-      <c r="J22" s="3">
+      <c r="I22">
+        <v>23</v>
+      </c>
+      <c r="J22">
         <v>178</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22">
         <v>81.7</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="5">
         <v>280.66666666666669</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22">
         <v>3704.5</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22">
         <v>4185.5</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22">
         <v>183.5</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22">
         <v>86.65</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R22">
         <v>188</v>
       </c>
-      <c r="S22" s="8">
+      <c r="S22" s="6">
         <v>12.71</v>
       </c>
-      <c r="T22" s="3">
+      <c r="T22">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="D23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23">
         <v>19.7</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23">
         <v>66</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="3">
+      <c r="H23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23">
         <v>24</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23">
         <v>191</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23">
         <v>82.1</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="5">
         <v>410</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23">
         <v>5116.5</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23">
         <v>5747</v>
       </c>
-      <c r="O23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P23" s="3">
+      <c r="O23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23">
         <v>1.125</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q23">
         <v>39.700000000000003</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R23">
         <v>186</v>
       </c>
-      <c r="S23" s="8">
+      <c r="S23" s="6">
         <v>11.7</v>
       </c>
-      <c r="T23" s="3">
+      <c r="T23">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="3">
+      <c r="D24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24">
         <v>20.100000000000001</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24">
         <v>68</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24">
         <v>24</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24">
         <v>191</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24">
         <v>81.8</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="5">
         <v>441.33333333333331</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24">
         <v>5163.5</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24">
         <v>6162.5</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24">
         <v>1.1949999999999998</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24">
         <v>190.5</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24">
         <v>47.599999999999994</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24">
         <v>191</v>
       </c>
-      <c r="S24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="T24" s="3">
+      <c r="S24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T24">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="3">
+      <c r="D25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25">
         <v>18.3</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25">
         <v>82</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25">
         <v>24</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25">
         <v>191</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25">
         <v>84</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L25" s="5">
         <v>432.66666666666669</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25">
         <v>4951</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25">
         <v>5755</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25">
         <v>1.165</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25">
         <v>163</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25">
         <v>39.6</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25">
         <v>178</v>
       </c>
-      <c r="S25" s="8">
+      <c r="S25" s="6">
         <v>10.78</v>
       </c>
-      <c r="T25" s="3">
+      <c r="T25">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="3">
+      <c r="D26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26">
         <v>19.600000000000001</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26">
         <v>53</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26">
         <v>24</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26">
         <v>178</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26">
         <v>84.3</v>
       </c>
-      <c r="L26" s="7">
+      <c r="L26" s="5">
         <v>455.66666666666669</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M26">
         <v>5294.5</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26">
         <v>6462.5</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26">
         <v>1.22</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P26">
         <v>214.5</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="Q26">
         <v>53.4</v>
       </c>
-      <c r="R26" s="3">
+      <c r="R26">
         <v>190</v>
       </c>
-      <c r="S26" s="8">
+      <c r="S26" s="6">
         <v>13.49</v>
       </c>
-      <c r="T26" s="3">
+      <c r="T26">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="3">
+      <c r="D27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27">
         <v>19</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27">
         <v>52</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27">
         <v>43</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27">
         <v>170</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27">
         <v>58.5</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27">
         <v>230</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27">
         <v>2543.5</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27">
         <v>3095.5</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27">
         <v>1.2149999999999999</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27">
         <v>106.5</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27">
         <v>41.4</v>
       </c>
-      <c r="R27" s="3">
+      <c r="R27">
         <v>181</v>
       </c>
-      <c r="S27" s="3">
+      <c r="S27">
         <v>10.15</v>
       </c>
-      <c r="T27" s="3">
+      <c r="T27">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="3">
+      <c r="D28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28">
         <v>19.5</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28">
         <v>68</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28">
         <v>29</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28">
         <v>176</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28">
         <v>79.099999999999994</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L28" s="5">
         <v>386.66666666666669</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28">
         <v>4694</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28">
         <v>5687</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28">
         <v>1.21</v>
       </c>
-      <c r="P28" s="3">
+      <c r="P28">
         <v>180.5</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28">
         <v>49.4</v>
       </c>
-      <c r="R28" s="3">
+      <c r="R28">
         <v>188</v>
       </c>
-      <c r="S28" s="3">
+      <c r="S28">
         <v>14.78</v>
       </c>
-      <c r="T28" s="3">
+      <c r="T28">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="A29" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="3">
+      <c r="D29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29">
         <v>19.2</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29">
         <v>66</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29">
         <v>29</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29">
         <v>176</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29">
         <v>78.7</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29">
         <v>390.66666666666669</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29">
         <v>4640.5</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29">
         <v>5604</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29">
         <v>1.2050000000000001</v>
       </c>
-      <c r="P29" s="3">
+      <c r="P29">
         <v>197</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="Q29">
         <v>187</v>
       </c>
-      <c r="R29" s="3">
+      <c r="R29">
         <v>187</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29">
         <v>15.16</v>
       </c>
-      <c r="T29" s="3">
+      <c r="T29">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="3">
+      <c r="D30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30">
         <v>20.5</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30">
         <v>74</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" s="3">
+      <c r="H30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30">
         <v>29</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30">
         <v>176</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30">
         <v>79.3</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30">
         <v>390</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30">
         <v>4614</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30">
         <v>5616.5</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30">
         <v>1.22</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P30">
         <v>175</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30">
         <v>46.6</v>
       </c>
-      <c r="R30" s="3">
+      <c r="R30">
         <v>186</v>
       </c>
-      <c r="S30" s="3">
+      <c r="S30">
         <v>14.6</v>
       </c>
-      <c r="T30" s="3">
+      <c r="T30">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="3">
+      <c r="D31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31">
         <v>19.8</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31">
         <v>67</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="3">
-        <v>23</v>
-      </c>
-      <c r="J31" s="3">
+      <c r="I31">
+        <v>23</v>
+      </c>
+      <c r="J31">
         <v>173</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31">
         <v>71.5</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="5">
         <v>267.67</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31">
         <v>3014.5</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31">
         <v>3435.5</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31">
         <v>1.1399999999999999</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P31">
         <v>98.5</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31">
         <v>35.299999999999997</v>
       </c>
-      <c r="R31" s="3">
+      <c r="R31">
         <v>182</v>
       </c>
-      <c r="S31" s="3">
+      <c r="S31">
         <v>12.15</v>
       </c>
-      <c r="T31" s="3">
+      <c r="T31">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="3">
+      <c r="D32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32">
         <v>19.7</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32">
         <v>67</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="3">
-        <v>23</v>
-      </c>
-      <c r="J32" s="3">
+      <c r="I32">
+        <v>23</v>
+      </c>
+      <c r="J32">
         <v>173</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32">
         <v>71.599999999999994</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32">
         <v>270</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32">
         <v>3103.5</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32">
         <v>3681</v>
       </c>
-      <c r="O32" s="3">
+      <c r="O32">
         <v>1.1850000000000001</v>
       </c>
-      <c r="P32" s="3">
+      <c r="P32">
         <v>113</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="Q32">
         <v>42.7</v>
       </c>
-      <c r="R32" s="3">
+      <c r="R32">
         <v>179</v>
       </c>
-      <c r="S32" s="3">
+      <c r="S32">
         <v>9.93</v>
       </c>
-      <c r="T32" s="3">
+      <c r="T32">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="3">
+      <c r="D33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33">
         <v>19.100000000000001</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33">
         <v>70</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" t="s">
         <v>43</v>
       </c>
-      <c r="I33" s="3">
-        <v>23</v>
-      </c>
-      <c r="J33" s="3">
+      <c r="I33">
+        <v>23</v>
+      </c>
+      <c r="J33">
         <v>173</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33">
         <v>71.5</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33">
         <v>270</v>
       </c>
-      <c r="M33" s="3">
+      <c r="M33">
         <v>3170.5</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33">
         <v>3637</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P33" s="3">
+      <c r="P33">
         <v>116.5</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="Q33">
         <v>41.95</v>
       </c>
-      <c r="R33" s="3">
+      <c r="R33">
         <v>175</v>
       </c>
-      <c r="S33" s="3">
+      <c r="S33">
         <v>11.01</v>
       </c>
-      <c r="T33" s="3">
+      <c r="T33">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="3">
+      <c r="D34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34">
         <v>19.8</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34">
         <v>52</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="3">
-        <v>23</v>
-      </c>
-      <c r="J34" s="3">
+      <c r="I34">
+        <v>23</v>
+      </c>
+      <c r="J34">
         <v>173</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34">
         <v>71.7</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34">
         <v>270</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34">
         <v>3093</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34">
         <v>3701</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34">
         <v>1.1949999999999998</v>
       </c>
-      <c r="P34" s="3">
+      <c r="P34">
         <v>117.5</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="Q34">
         <v>42.4</v>
       </c>
-      <c r="R34" s="3">
+      <c r="R34">
         <v>179</v>
       </c>
-      <c r="S34" s="3">
+      <c r="S34">
         <v>10.72</v>
       </c>
-      <c r="T34" s="3">
+      <c r="T34">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="3">
+      <c r="D35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35">
         <v>19.8</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35">
         <v>67</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="H35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35">
         <v>24</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35">
         <v>178</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35">
         <v>64.099999999999994</v>
       </c>
-      <c r="L35" s="7">
+      <c r="L35" s="5">
         <v>318.33333333333331</v>
       </c>
-      <c r="M35" s="3">
+      <c r="M35">
         <v>3576.5</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35">
         <v>4025</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O35">
         <v>1.125</v>
       </c>
-      <c r="P35" s="3">
+      <c r="P35">
         <v>112</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="Q35">
         <v>32.200000000000003</v>
       </c>
-      <c r="R35" s="3">
+      <c r="R35">
         <v>168</v>
       </c>
-      <c r="S35" s="3">
+      <c r="S35">
         <v>6.43</v>
       </c>
-      <c r="T35" s="3">
+      <c r="T35">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="3">
+      <c r="D36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36">
         <v>19.7</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36">
         <v>67</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36">
         <v>24</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36">
         <v>178</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36">
         <v>65</v>
       </c>
-      <c r="L36" s="7">
+      <c r="L36" s="5">
         <v>318.33333333333331</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M36">
         <v>3713</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36">
         <v>4162</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36">
         <v>1.1200000000000001</v>
       </c>
-      <c r="P36" s="3">
+      <c r="P36">
         <v>104.5</v>
       </c>
-      <c r="Q36" s="3">
+      <c r="Q36">
         <v>30.349999999999998</v>
       </c>
-      <c r="R36" s="3">
+      <c r="R36">
         <v>169</v>
       </c>
-      <c r="S36" s="3">
+      <c r="S36">
         <v>6.68</v>
       </c>
-      <c r="T36" s="3">
+      <c r="T36">
         <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="3">
+      <c r="D37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37">
         <v>19.8</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37">
         <v>67</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="3">
-        <v>23</v>
-      </c>
-      <c r="J37" s="3">
+      <c r="H37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37">
+        <v>23</v>
+      </c>
+      <c r="J37">
         <v>176</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37">
         <v>72.599999999999994</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37">
         <v>390</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M37">
         <v>4332.5</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37">
         <v>4716</v>
       </c>
-      <c r="O37" s="3">
+      <c r="O37">
         <v>1.0900000000000001</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P37">
         <v>113.5</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="Q37">
         <v>38.599999999999994</v>
       </c>
-      <c r="R37" s="3">
+      <c r="R37">
         <v>194</v>
       </c>
-      <c r="S37" s="3">
+      <c r="S37">
         <v>9.4499999999999993</v>
       </c>
-      <c r="T37" s="3">
+      <c r="T37">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="3">
+      <c r="D38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38">
         <v>19.7</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38">
         <v>67</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" s="3">
-        <v>23</v>
-      </c>
-      <c r="J38" s="3">
+      <c r="H38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38">
+        <v>23</v>
+      </c>
+      <c r="J38">
         <v>176</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38">
         <v>72.599999999999994</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38">
         <v>390</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M38">
         <v>4362</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38">
         <v>4819.5</v>
       </c>
-      <c r="O38" s="3">
+      <c r="O38">
         <v>1.105</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P38">
         <v>127.5</v>
       </c>
-      <c r="Q38" s="3">
+      <c r="Q38">
         <v>43.2</v>
       </c>
-      <c r="R38" s="3">
+      <c r="R38">
         <v>190</v>
       </c>
-      <c r="S38" s="3">
+      <c r="S38">
         <v>9.07</v>
       </c>
-      <c r="T38" s="3">
+      <c r="T38">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="3">
+      <c r="D39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39">
         <v>19.100000000000001</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39">
         <v>70</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="3">
-        <v>23</v>
-      </c>
-      <c r="J39" s="3">
+      <c r="H39" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39">
+        <v>23</v>
+      </c>
+      <c r="J39">
         <v>176</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39">
         <v>72.599999999999994</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39">
         <v>440.66666666666669</v>
       </c>
-      <c r="M39" s="3">
+      <c r="M39">
         <v>4737</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39">
         <v>5640</v>
       </c>
-      <c r="O39" s="3">
+      <c r="O39">
         <v>1.1949999999999998</v>
       </c>
-      <c r="P39" s="3">
+      <c r="P39">
         <v>201.5</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="Q39">
         <v>68.95</v>
       </c>
-      <c r="R39" s="3">
+      <c r="R39">
         <v>202</v>
       </c>
-      <c r="S39" s="3">
+      <c r="S39">
         <v>19.62</v>
       </c>
-      <c r="T39" s="3">
+      <c r="T39">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="3">
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40">
         <v>18.3</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40">
         <v>51</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="H40" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40">
         <v>26</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40">
         <v>187</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40">
         <v>88.8</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40">
         <v>341</v>
       </c>
-      <c r="M40" s="3">
+      <c r="M40">
         <v>4634.5</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40">
         <v>5453</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40">
         <v>1.1749999999999998</v>
       </c>
-      <c r="P40" s="3">
+      <c r="P40">
         <v>201.5</v>
       </c>
-      <c r="Q40" s="3">
+      <c r="Q40">
         <v>54.8</v>
       </c>
-      <c r="R40" s="3">
+      <c r="R40">
         <v>194</v>
       </c>
-      <c r="S40" s="3">
+      <c r="S40">
         <v>15.43</v>
       </c>
-      <c r="T40" s="3">
+      <c r="T40">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="3">
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41">
         <v>18</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41">
         <v>70</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41" s="3">
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41">
         <v>26</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41">
         <v>187</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41">
         <v>90.1</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41">
         <v>344.33333333333331</v>
       </c>
-      <c r="M41" s="3">
+      <c r="M41">
         <v>4606.5</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41">
         <v>5312</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O41">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P41">
         <v>182.5</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="Q41">
         <v>49.599999999999994</v>
       </c>
-      <c r="R41" s="3">
+      <c r="R41">
         <v>194</v>
       </c>
-      <c r="S41" s="3">
+      <c r="S41">
         <v>12.97</v>
       </c>
-      <c r="T41" s="3">
+      <c r="T41">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="3">
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42">
         <v>18.399999999999999</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42">
         <v>70</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" s="3">
+      <c r="H42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42">
         <v>26</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42">
         <v>187</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42">
         <v>90</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42">
         <v>354.33333333333331</v>
       </c>
-      <c r="M42" s="3">
+      <c r="M42">
         <v>4540.5</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42">
         <v>5324.5</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O42">
         <v>1.17</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P42">
         <v>176</v>
       </c>
-      <c r="Q42" s="3">
+      <c r="Q42">
         <v>48.349999999999994</v>
       </c>
-      <c r="R42" s="3">
+      <c r="R42">
         <v>194</v>
       </c>
-      <c r="S42" s="3">
+      <c r="S42">
         <v>14.77</v>
       </c>
-      <c r="T42" s="3">
+      <c r="T42">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+      <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="3">
+      <c r="D43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43">
         <v>18.3</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43">
         <v>51</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43" s="3">
+      <c r="H43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43">
         <v>27</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43">
         <v>180</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43">
         <v>68.5</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43">
         <v>385.33333333333331</v>
       </c>
-      <c r="M43" s="3">
+      <c r="M43">
         <v>4556.5</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43">
         <v>5129</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O43">
         <v>1.125</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P43">
         <v>176.5</v>
       </c>
-      <c r="Q43" s="3">
+      <c r="Q43">
         <v>48.95</v>
       </c>
-      <c r="R43" s="3">
+      <c r="R43">
         <v>191</v>
       </c>
-      <c r="S43" s="3">
+      <c r="S43">
         <v>15.78</v>
       </c>
-      <c r="T43" s="3">
+      <c r="T43">
         <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="3">
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44">
         <v>17.899999999999999</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44">
         <v>70</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I44" s="3">
+      <c r="H44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44">
         <v>27</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44">
         <v>180</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44">
         <v>68.8</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44">
         <v>380</v>
       </c>
-      <c r="M44" s="3">
+      <c r="M44">
         <v>4561.5</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44">
         <v>5071</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O44">
         <v>1.115</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P44">
         <v>187.5</v>
       </c>
-      <c r="Q44" s="3">
+      <c r="Q44">
         <v>69.55</v>
       </c>
-      <c r="R44" s="3">
+      <c r="R44">
         <v>188</v>
       </c>
-      <c r="S44" s="3">
+      <c r="S44">
         <v>16.16</v>
       </c>
-      <c r="T44" s="3">
+      <c r="T44">
         <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F45" s="3">
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45">
         <v>18.7</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45">
         <v>65</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="H45" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45">
         <v>27</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45">
         <v>180</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45">
         <v>69.2</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45">
         <v>371.66666666666669</v>
       </c>
-      <c r="M45" s="3">
+      <c r="M45">
         <v>4437</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45">
         <v>4991.5</v>
       </c>
-      <c r="O45" s="3">
+      <c r="O45">
         <v>1.125</v>
       </c>
-      <c r="P45" s="3">
+      <c r="P45">
         <v>164</v>
       </c>
-      <c r="Q45" s="3">
+      <c r="Q45">
         <v>43.35</v>
       </c>
-      <c r="R45" s="3">
+      <c r="R45">
         <v>187</v>
       </c>
-      <c r="S45" s="3">
+      <c r="S45">
         <v>13.93</v>
       </c>
-      <c r="T45" s="3">
+      <c r="T45">
         <v>18</v>
       </c>
     </row>
@@ -3163,10 +3160,10 @@
       <c r="C46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="6" t="s">
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F46" s="2">
@@ -3216,126 +3213,126 @@
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="A47" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="3">
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47">
         <v>18</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47">
         <v>69</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I47" s="3">
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47">
         <v>27</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47">
         <v>187</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47">
         <v>103.9</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47">
         <v>305</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47">
         <v>4350.5</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47">
         <v>5034</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47">
         <v>1.1549999999999998</v>
       </c>
-      <c r="P47" s="3">
+      <c r="P47">
         <v>206</v>
       </c>
-      <c r="Q47" s="3">
+      <c r="Q47">
         <v>47.3</v>
       </c>
-      <c r="R47" s="3">
+      <c r="R47">
         <v>183</v>
       </c>
-      <c r="S47" s="3">
+      <c r="S47">
         <v>9.25</v>
       </c>
-      <c r="T47" s="3">
+      <c r="T47">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="A48" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F48" s="3">
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48">
         <v>18</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48">
         <v>69</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I48" s="3">
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48">
         <v>27</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48">
         <v>187</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48">
         <v>103.6</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48">
         <v>280.33333333333331</v>
       </c>
-      <c r="M48" s="3">
+      <c r="M48">
         <v>3818.5</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48">
         <v>4471</v>
       </c>
-      <c r="O48" s="3">
+      <c r="O48">
         <v>1.1749999999999998</v>
       </c>
-      <c r="P48" s="3">
+      <c r="P48">
         <v>196</v>
       </c>
-      <c r="Q48" s="3">
+      <c r="Q48">
         <v>63.85</v>
       </c>
-      <c r="R48" s="3">
+      <c r="R48">
         <v>180</v>
       </c>
-      <c r="S48" s="3">
+      <c r="S48">
         <v>11.1</v>
       </c>
-      <c r="T48" s="3">
+      <c r="T48">
         <v>16</v>
       </c>
     </row>
@@ -3349,10 +3346,10 @@
       <c r="C49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="6" t="s">
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F49" s="2">
@@ -3402,126 +3399,126 @@
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+      <c r="A50" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
         <v>21</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F50" s="3">
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50">
         <v>18</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50">
         <v>70</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I50" s="3">
-        <v>22</v>
-      </c>
-      <c r="J50" s="3">
+      <c r="H50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50">
+        <v>22</v>
+      </c>
+      <c r="J50">
         <v>191</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50">
         <v>82.1</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50">
         <v>383.66666666666669</v>
       </c>
-      <c r="M50" s="3">
+      <c r="M50">
         <v>4872</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50">
         <v>5276.5</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O50">
         <v>1.085</v>
       </c>
-      <c r="P50" s="3">
+      <c r="P50">
         <v>192</v>
       </c>
-      <c r="Q50" s="3">
+      <c r="Q50">
         <v>80.099999999999994</v>
       </c>
-      <c r="R50" s="3">
+      <c r="R50">
         <v>187</v>
       </c>
-      <c r="S50" s="3">
+      <c r="S50">
         <v>8.9700000000000006</v>
       </c>
-      <c r="T50" s="3">
+      <c r="T50">
         <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F51" s="3">
+      <c r="D51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51">
         <v>18</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51">
         <v>69</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I51" s="3">
-        <v>22</v>
-      </c>
-      <c r="J51" s="3">
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51">
+        <v>22</v>
+      </c>
+      <c r="J51">
         <v>191</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51">
         <v>82.8</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51">
         <v>379.33333333333331</v>
       </c>
-      <c r="M51" s="3">
+      <c r="M51">
         <v>5050</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51">
         <v>5561</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O51">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P51" s="3">
+      <c r="P51">
         <v>190.5</v>
       </c>
-      <c r="Q51" s="3">
+      <c r="Q51">
         <v>68.8</v>
       </c>
-      <c r="R51" s="3">
+      <c r="R51">
         <v>181</v>
       </c>
-      <c r="S51" s="3">
+      <c r="S51">
         <v>9.07</v>
       </c>
-      <c r="T51" s="3">
+      <c r="T51">
         <v>20</v>
       </c>
     </row>

</xml_diff>